<commit_message>
Updated noise dB SPL to be 60db SPL
Accounting for frequency response curve of Sennheiser HD280
</commit_message>
<xml_diff>
--- a/Auditory Tone Detection Task/questConditionsFile.xlsx
+++ b/Auditory Tone Detection Task/questConditionsFile.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonhe/Dropbox/Documents/GitHub/Open-source Auditory Tone Detection (OSATD) Task/Auditory Tone Detection Task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W2032175\Documents\GitHub\Open-source-Auditory-Tone-Detection-Task\Auditory Tone Detection Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4046F83E-9399-604D-82E3-C43C88CB5FC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD5EBC-7AE8-4739-9A58-5DE788432798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{39D40CD4-76BC-4DB8-8C0A-D42107145D07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39D40CD4-76BC-4DB8-8C0A-D42107145D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -422,16 +425,16 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,15 +469,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>80</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <f>0.4*B2</f>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>0.63</v>
@@ -492,13 +496,13 @@
         <v>0.01</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="L2" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated Quest conditions file
Reduced the starting value for the questCondtions file from 80 to 60, as some participants are not thresholding for the quiet task.
</commit_message>
<xml_diff>
--- a/Auditory Tone Detection Task/questConditionsFile.xlsx
+++ b/Auditory Tone Detection Task/questConditionsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W2032175\Documents\GitHub\Open-source-Auditory-Tone-Detection-Task\Auditory Tone Detection Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonhe/Documents/Documents - Jason's iCloud/Work/GitHub/HeJasonL/Open-source-Auditory-Tone-Detection-Task/Auditory Tone Detection Task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD5EBC-7AE8-4739-9A58-5DE788432798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429C23E5-2F62-8040-9DC7-248F1F4BC48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39D40CD4-76BC-4DB8-8C0A-D42107145D07}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{39D40CD4-76BC-4DB8-8C0A-D42107145D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,16 +425,16 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,16 +469,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <f>0.4*B2</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>0.63</v>

</xml_diff>